<commit_message>
Fixed RX & TX Issue #5 Switched RX & TX of FT232RL and ESP 32.
</commit_message>
<xml_diff>
--- a/Dokumentation/Bestellliste_PSP20_Hardware.xlsx
+++ b/Dokumentation/Bestellliste_PSP20_Hardware.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DL7MLP\Desktop\Sees\PSP20\Hardware\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D33DBB-44C4-4FCD-870D-F25711F374C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A365320-94B0-413A-B74D-8BDB2B7EC067}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30750" yWindow="-10815" windowWidth="13500" windowHeight="20835" xr2:uid="{BECEF3FB-4803-4E7A-92DF-8A75AD85CD69}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BECEF3FB-4803-4E7A-92DF-8A75AD85CD69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="42">
   <si>
     <t>Anzahl</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Achtung 10er Pack als Bestelleinheit. 2500 Stück gesamt. 250 Bestelleinheiten.</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -574,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155ABF72-82D7-4794-95E6-AE95DC9723A2}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +593,7 @@
     <col min="8" max="8" width="70.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>60</v>
       </c>
@@ -633,8 +636,11 @@
       <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
@@ -654,8 +660,11 @@
       <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>60</v>
       </c>
@@ -675,8 +684,11 @@
       <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>200</v>
       </c>
@@ -696,8 +708,11 @@
       <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>200</v>
       </c>
@@ -717,8 +732,11 @@
       <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>200</v>
       </c>
@@ -738,8 +756,11 @@
       <c r="G7" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2500</v>
       </c>
@@ -759,8 +780,11 @@
       <c r="G8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2500</v>
       </c>
@@ -780,8 +804,11 @@
       <c r="G9" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>60</v>
       </c>
@@ -801,8 +828,11 @@
       <c r="G10" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>60</v>
       </c>
@@ -822,8 +852,11 @@
       <c r="G11" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>200</v>
       </c>
@@ -843,8 +876,11 @@
       <c r="G12" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>100</v>
       </c>
@@ -864,8 +900,11 @@
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>200</v>
       </c>
@@ -885,8 +924,11 @@
       <c r="G14" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>160</v>
       </c>
@@ -906,8 +948,11 @@
       <c r="G15" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>150</v>
       </c>
@@ -927,8 +972,11 @@
       <c r="G16" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>400</v>
       </c>
@@ -948,8 +996,11 @@
       <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>60</v>
       </c>
@@ -969,8 +1020,11 @@
       <c r="G18" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>60</v>
       </c>
@@ -990,8 +1044,11 @@
       <c r="G19" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>60</v>
       </c>
@@ -1011,8 +1068,11 @@
       <c r="G20" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>60</v>
       </c>
@@ -1032,8 +1092,11 @@
       <c r="G21" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>60</v>
       </c>
@@ -1053,8 +1116,11 @@
       <c r="G22" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>60</v>
       </c>
@@ -1074,8 +1140,11 @@
       <c r="G23" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>250</v>
       </c>
@@ -1098,8 +1167,11 @@
       <c r="H24" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>60</v>
       </c>
@@ -1119,8 +1191,11 @@
       <c r="G25" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>

</xml_diff>